<commit_message>
change linkefin google form (erreur ds le formulaire)
</commit_message>
<xml_diff>
--- a/src/premium/Config/filtres_13.xlsx
+++ b/src/premium/Config/filtres_13.xlsx
@@ -1,37 +1,129 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/remyadda/Desktop/AD/Projets/AD_serveur/src/premium/Config/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA3816D-182C-3A48-BB77-013D777E22B4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+  <si>
+    <t>Horodateur</t>
+  </si>
+  <si>
+    <t>Nom - Prénom - Nom société</t>
+  </si>
+  <si>
+    <t>NIVEAU DE RELATION</t>
+  </si>
+  <si>
+    <t>ZONE GÉOGRAPHIQUE</t>
+  </si>
+  <si>
+    <t>SECTEUR</t>
+  </si>
+  <si>
+    <t>LANGUE</t>
+  </si>
+  <si>
+    <t>ÉCOLE</t>
+  </si>
+  <si>
+    <t>HIÉRARCHIE</t>
+  </si>
+  <si>
+    <t>ANCIENNETÉ DU POSTE</t>
+  </si>
+  <si>
+    <t>ANCIENNETÉ D'ENTREPRISE</t>
+  </si>
+  <si>
+    <t>FONCTION</t>
+  </si>
+  <si>
+    <t>TITRE</t>
+  </si>
+  <si>
+    <t>EXPERIENCE</t>
+  </si>
+  <si>
+    <t>ENTREPRISE</t>
+  </si>
+  <si>
+    <t>EFFECTIF</t>
+  </si>
+  <si>
+    <t>TYPE D'ENTREPRISE</t>
+  </si>
+  <si>
+    <t>2021/01/14 12:10:46 PM UTC+2</t>
+  </si>
+  <si>
+    <t>Bonan - Dan - Troof SAS</t>
+  </si>
+  <si>
+    <t>Relations de 3e niveau et plus</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Articles de luxe et bijouterie;Confection et mode;Matériel informatique;Médecines alternatives;Vins et spiritueux</t>
+  </si>
+  <si>
+    <t>Français</t>
+  </si>
+  <si>
+    <t>Propriétaire;PDG;Directeur;Cadre supérieur</t>
+  </si>
+  <si>
+    <t>Entre 3 et 5 ans;Entre 6 et 10 ans;Plus de 10 ans</t>
+  </si>
+  <si>
+    <t>De 3 à 5 ans;De 6 à 10 ans;Plus de 10 ans</t>
+  </si>
+  <si>
+    <t>Indépendant;1-10;11-50;51-200</t>
+  </si>
+  <si>
+    <t>Société civile/Société commerciale/Autres types de sociétés;Société de personnes (associés);Indépendant;Propriété propre</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,10 +138,18 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -57,15 +157,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -353,168 +462,116 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="88" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="37.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="25.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Horodateur</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Nom - Prénom - Nom société</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>NIVEAU DE RELATION</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>ZONE GÉOGRAPHIQUE</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>SECTEUR</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>LANGUE</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>ÉCOLE</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>HIÉRARCHIE</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>ANCIENNETÉ DU POSTE</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>ANCIENNETÉ D'ENTREPRISE</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>FONCTION</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>TITRE</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>EXPERIENCE</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>ENTREPRISE</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>EFFECTIF</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>TYPE D'ENTREPRISE</t>
-        </is>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
         <v>4</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2021/01/14 12:10:46 PM UTC+2</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Bonan - Dan - Troof SAS</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Relations de 3e niveau et plus</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>France</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Articles de luxe et bijouterie;Confection et mode;Matériel informatique;Médecines alternatives;Vins et spiritueux</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Français</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Propriétaire;PDG;Directeur;Cadre supérieur</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>Entre 3 et 5 ans;Entre 6 et 10 ans;Plus de 10 ans</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>Entre 3 et 5 ans;Entre 6 et 10 ans;Plus de 10 ans</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>De 3 à 5 ans;De 6 à 10 ans;Plus de 10 ans</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr"/>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>Indépendant;1-10;11-50;51-200</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>Indépendant;1-10;11-50;51-200</t>
-        </is>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>